<commit_message>
Penambahan data PC di file data pc.xlsx
</commit_message>
<xml_diff>
--- a/data pc.xlsx
+++ b/data pc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="126">
   <si>
     <t>Daftar PC</t>
   </si>
@@ -70,7 +70,7 @@
     <t>Marketing</t>
   </si>
   <si>
-    <t>MSI H61M P28</t>
+    <t>MSI H61M-P28</t>
   </si>
   <si>
     <t>Core i3 - 3210, 3.2GHz</t>
@@ -82,7 +82,7 @@
     <t>Intel H61</t>
   </si>
   <si>
-    <t>Samsung 19 Inch</t>
+    <t>Samsung 19"</t>
   </si>
   <si>
     <t>Logitech</t>
@@ -124,7 +124,7 @@
     <t>Cost Control</t>
   </si>
   <si>
-    <t>MSI H61M E33 Combo</t>
+    <t>MSI H61M-E33 Combo</t>
   </si>
   <si>
     <t>Dual Core E5700, 3GHz</t>
@@ -142,7 +142,7 @@
     <t>dual Core E5700, 3GHz</t>
   </si>
   <si>
-    <t>LG 19 Inch</t>
+    <t>LG 19"</t>
   </si>
   <si>
     <t>logitech</t>
@@ -172,7 +172,7 @@
     <t>1 GB</t>
   </si>
   <si>
-    <t>Acer 19 Inch</t>
+    <t>Acer 19"</t>
   </si>
   <si>
     <t>Lt. 5</t>
@@ -181,13 +181,16 @@
     <t>Intan</t>
   </si>
   <si>
+    <t>ASRock H61M-VG3</t>
+  </si>
+  <si>
     <t>Lt. 6</t>
   </si>
   <si>
     <t>Alisa</t>
   </si>
   <si>
-    <t>MSI G31 TM P31</t>
+    <t>MSI G31TM-P31</t>
   </si>
   <si>
     <t>dual Core E5500, 2.8GHz</t>
@@ -202,7 +205,7 @@
     <t>Engineering</t>
   </si>
   <si>
-    <t>MSI H61M E33</t>
+    <t>MSI H61M-E33</t>
   </si>
   <si>
     <t>Core i3 - 2100, 3.1GHz</t>
@@ -223,7 +226,7 @@
     <t>8 GB</t>
   </si>
   <si>
-    <t>Dell 19 Inch</t>
+    <t>Dell 19"</t>
   </si>
   <si>
     <t>Print Server</t>
@@ -238,7 +241,7 @@
     <t>Utomo</t>
   </si>
   <si>
-    <t>HP 23 Inch</t>
+    <t>HP 23"</t>
   </si>
   <si>
     <t>HP</t>
@@ -256,127 +259,139 @@
     <t>Nvidia Gforce GT730 2GB</t>
   </si>
   <si>
-    <t>Win 10 66Bit</t>
+    <t>Win 10 64Bit</t>
   </si>
   <si>
     <t>Didit</t>
   </si>
   <si>
-    <t>HP Prodesk 400 G5</t>
-  </si>
-  <si>
     <t>Core i7 3.6GHz HZ71</t>
   </si>
   <si>
-    <t>9 GB</t>
-  </si>
-  <si>
-    <t>Nvidia Gforce GT730 3GB</t>
-  </si>
-  <si>
-    <t>HP 24 Inch</t>
-  </si>
-  <si>
     <t>Robert</t>
   </si>
   <si>
-    <t>HP Prodesk 400 G6</t>
-  </si>
-  <si>
     <t>Core i7 3.6GHz HZ72</t>
   </si>
   <si>
-    <t>Nvidia Gforce GT730 4GB</t>
-  </si>
-  <si>
-    <t>HP 25 Inch</t>
-  </si>
-  <si>
     <t>Kiki</t>
   </si>
   <si>
-    <t>HP Prodesk 400 G7</t>
-  </si>
-  <si>
     <t>Core i7 3.6GHz HZ73</t>
   </si>
   <si>
-    <t>11 GB</t>
-  </si>
-  <si>
-    <t>Nvidia Gforce GT730 5GB</t>
-  </si>
-  <si>
-    <t>HP 26 Inch</t>
-  </si>
-  <si>
     <t>Andy</t>
   </si>
   <si>
-    <t>HP Prodesk 400 G8</t>
-  </si>
-  <si>
     <t>Core i7 3.6GHz HZ74</t>
   </si>
   <si>
-    <t>Nvidia Gforce GT730 6GB</t>
-  </si>
-  <si>
-    <t>HP 27 Inch</t>
-  </si>
-  <si>
     <t>Fega</t>
   </si>
   <si>
-    <t>HP Prodesk 400 G9</t>
-  </si>
-  <si>
     <t>Core i7 3.6GHz HZ75</t>
   </si>
   <si>
-    <t>13 GB</t>
-  </si>
-  <si>
-    <t>Nvidia Gforce GT730 7GB</t>
-  </si>
-  <si>
-    <t>HP 28 Inch</t>
-  </si>
-  <si>
     <t>Kadek</t>
   </si>
   <si>
-    <t>HP Prodesk 400 G10</t>
-  </si>
-  <si>
     <t>Core i7 3.6GHz HZ76</t>
   </si>
   <si>
-    <t>14 GB</t>
-  </si>
-  <si>
-    <t>Nvidia Gforce GT730 8GB</t>
-  </si>
-  <si>
-    <t>HP 29 Inch</t>
-  </si>
-  <si>
     <t>laksono</t>
   </si>
   <si>
-    <t>HP Prodesk 400 G11</t>
-  </si>
-  <si>
     <t>Core i7 3.6GHz HZ77</t>
   </si>
   <si>
-    <t>15 GB</t>
-  </si>
-  <si>
-    <t>Nvidia Gforce GT730 9GB</t>
-  </si>
-  <si>
-    <t>HP 30 Inch</t>
+    <t>Eko</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>MSI G41M-P28</t>
+  </si>
+  <si>
+    <t>2GB</t>
+  </si>
+  <si>
+    <t>Intel G41</t>
+  </si>
+  <si>
+    <t>Lt. 1</t>
+  </si>
+  <si>
+    <t>Azis</t>
+  </si>
+  <si>
+    <t>Dual Core E5400</t>
+  </si>
+  <si>
+    <t>Dedi</t>
+  </si>
+  <si>
+    <t>1GB</t>
+  </si>
+  <si>
+    <t>Yuli</t>
+  </si>
+  <si>
+    <t>ASUSTek P5G41T-MLX3 Plus</t>
+  </si>
+  <si>
+    <t>Dual Core E5500</t>
+  </si>
+  <si>
+    <t>Jefri</t>
+  </si>
+  <si>
+    <t>ECS H61H2-M13</t>
+  </si>
+  <si>
+    <t>Pentium G620</t>
+  </si>
+  <si>
+    <t>Tanti</t>
+  </si>
+  <si>
+    <t>PPIC</t>
+  </si>
+  <si>
+    <t>MSI G41-P28</t>
+  </si>
+  <si>
+    <t>Tengah</t>
+  </si>
+  <si>
+    <t>Dyah</t>
+  </si>
+  <si>
+    <t>4GB</t>
+  </si>
+  <si>
+    <t>Wito</t>
+  </si>
+  <si>
+    <t>MTC</t>
+  </si>
+  <si>
+    <t>ASRock H61M-VS4</t>
+  </si>
+  <si>
+    <t>Mei</t>
+  </si>
+  <si>
+    <t>FO</t>
+  </si>
+  <si>
+    <t>Intel DG41WV</t>
+  </si>
+  <si>
+    <t>Dual Core E5800</t>
+  </si>
+  <si>
+    <t>LG 19”</t>
   </si>
 </sst>
 </file>
@@ -384,18 +399,24 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_(* #.##0_);_(* \(#.##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_(* #.##0_);_(* \(#.##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_(* #,###.##000_);_(* \(#,###.##000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -405,8 +426,122 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -421,126 +556,12 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -551,6 +572,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -563,180 +608,156 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -745,11 +766,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="hair">
+        <color indexed="8"/>
+      </left>
+      <right style="hair">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -759,6 +801,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -787,17 +844,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -812,195 +878,174 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1050,6 +1095,7 @@
     <cellStyle name="Accent6" xfId="46" builtinId="49"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="Excel Built-in Normal" xfId="49"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1318,10 +1364,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1333,7 +1379,8 @@
     <col min="5" max="5" width="21.4285714285714" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
     <col min="7" max="7" width="19.5714285714286" customWidth="1"/>
-    <col min="9" max="9" width="18.1428571428571" customWidth="1"/>
+    <col min="8" max="8" width="8.28571428571429" customWidth="1"/>
+    <col min="9" max="9" width="12.5714285714286" customWidth="1"/>
     <col min="10" max="10" width="9.42857142857143" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
@@ -1748,7 +1795,7 @@
         <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
         <v>37</v>
@@ -1778,7 +1825,7 @@
         <v>163</v>
       </c>
       <c r="N10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O10" t="s">
         <v>27</v>
@@ -1789,22 +1836,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
         <v>51</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H11">
         <v>250</v>
@@ -1825,7 +1872,7 @@
         <v>162</v>
       </c>
       <c r="N11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="O11" t="s">
         <v>27</v>
@@ -1836,22 +1883,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H12">
         <v>250</v>
@@ -1883,19 +1930,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
         <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G13" t="s">
         <v>38</v>
@@ -1904,7 +1951,7 @@
         <v>250</v>
       </c>
       <c r="I13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J13" t="s">
         <v>23</v>
@@ -1930,19 +1977,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
         <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
         <v>21</v>
@@ -1954,7 +2001,7 @@
         <v>22</v>
       </c>
       <c r="J14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K14" t="s">
         <v>24</v>
@@ -1977,34 +2024,34 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H15">
         <v>250</v>
       </c>
       <c r="I15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L15" t="s">
         <v>25</v>
@@ -2024,37 +2071,37 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H16">
         <v>1000</v>
       </c>
       <c r="I16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M16">
         <v>17</v>
@@ -2071,37 +2118,37 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
         <v>83</v>
       </c>
       <c r="F17" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="G17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H17">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="I17" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="J17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M17">
         <v>36</v>
@@ -2118,37 +2165,37 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="G18" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H18">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="I18" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="J18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M18">
         <v>27</v>
@@ -2165,37 +2212,37 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F19" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="H19">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="I19" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="J19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M19">
         <v>24</v>
@@ -2212,37 +2259,37 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="E20" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="H20">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="I20" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="J20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M20">
         <v>12</v>
@@ -2259,37 +2306,37 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="E21" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="F21" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="G21" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="H21">
-        <v>1005</v>
+        <v>1000</v>
       </c>
       <c r="I21" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="J21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M21">
         <v>31</v>
@@ -2306,37 +2353,37 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="E22" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="F22" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="G22" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="H22">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="I22" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="J22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M22">
         <v>15</v>
@@ -2353,37 +2400,37 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="E23" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="G23" t="s">
-        <v>119</v>
+        <v>80</v>
       </c>
       <c r="H23">
-        <v>1007</v>
+        <v>1000</v>
       </c>
       <c r="I23" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="J23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M23">
         <v>38</v>
@@ -2392,6 +2439,446 @@
         <v>26</v>
       </c>
       <c r="O23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15">
+      <c r="B31" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H31" s="2">
+        <v>320</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L31" t="s">
+        <v>39</v>
+      </c>
+      <c r="M31">
+        <v>85</v>
+      </c>
+      <c r="N31" t="s">
+        <v>101</v>
+      </c>
+      <c r="O31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15">
+      <c r="B32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H32" s="2">
+        <v>250</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L32" t="s">
+        <v>39</v>
+      </c>
+      <c r="M32">
+        <v>84</v>
+      </c>
+      <c r="N32" t="s">
+        <v>101</v>
+      </c>
+      <c r="O32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15">
+      <c r="B33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H33" s="2">
+        <v>250</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L33" t="s">
+        <v>39</v>
+      </c>
+      <c r="M33">
+        <v>83</v>
+      </c>
+      <c r="N33" t="s">
+        <v>101</v>
+      </c>
+      <c r="O33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15">
+      <c r="B34" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H34" s="2">
+        <v>250</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M34">
+        <v>84</v>
+      </c>
+      <c r="N34" t="s">
+        <v>101</v>
+      </c>
+      <c r="O34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15">
+      <c r="B35" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" s="2">
+        <v>250</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L35" t="s">
+        <v>39</v>
+      </c>
+      <c r="M35">
+        <v>86</v>
+      </c>
+      <c r="N35" t="s">
+        <v>101</v>
+      </c>
+      <c r="O35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15">
+      <c r="B37" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" t="s">
+        <v>37</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H37">
+        <v>250</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L37" t="s">
+        <v>33</v>
+      </c>
+      <c r="M37">
+        <v>76</v>
+      </c>
+      <c r="N37" t="s">
+        <v>101</v>
+      </c>
+      <c r="O37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15">
+      <c r="B38" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H38">
+        <v>250</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L38" t="s">
+        <v>39</v>
+      </c>
+      <c r="M38">
+        <v>78</v>
+      </c>
+      <c r="N38" t="s">
+        <v>101</v>
+      </c>
+      <c r="O38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15">
+      <c r="B39" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E39" t="s">
+        <v>37</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H39">
+        <v>320</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L39" t="s">
+        <v>25</v>
+      </c>
+      <c r="M39">
+        <v>189</v>
+      </c>
+      <c r="N39" t="s">
+        <v>101</v>
+      </c>
+      <c r="O39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15">
+      <c r="B41" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E41" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41">
+        <v>500</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L41" t="s">
+        <v>25</v>
+      </c>
+      <c r="M41">
+        <v>113</v>
+      </c>
+      <c r="N41" t="s">
+        <v>101</v>
+      </c>
+      <c r="O41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15">
+      <c r="B43" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H43">
+        <v>250</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L43" t="s">
+        <v>39</v>
+      </c>
+      <c r="M43">
+        <v>233</v>
+      </c>
+      <c r="N43" t="s">
+        <v>101</v>
+      </c>
+      <c r="O43" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
penambahan data pc baru
</commit_message>
<xml_diff>
--- a/data pc.xlsx
+++ b/data pc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="152">
   <si>
     <t>Daftar PC</t>
   </si>
@@ -76,7 +76,7 @@
     <t>Core i3 - 3210, 3.2GHz</t>
   </si>
   <si>
-    <t>10 GB</t>
+    <t>10GB</t>
   </si>
   <si>
     <t>Intel H61</t>
@@ -109,7 +109,7 @@
     <t>Pentium G2030, 3GHz</t>
   </si>
   <si>
-    <t>2 GB</t>
+    <t>2GB</t>
   </si>
   <si>
     <t>Vorte</t>
@@ -154,39 +154,27 @@
     <t>Purchasing</t>
   </si>
   <si>
-    <t>Lt. 3</t>
-  </si>
-  <si>
     <t>Ferly</t>
   </si>
   <si>
     <t>A4Tech</t>
   </si>
   <si>
-    <t>Lt. 4</t>
-  </si>
-  <si>
     <t>Ana</t>
   </si>
   <si>
-    <t>1 GB</t>
+    <t>1GB</t>
   </si>
   <si>
     <t>Acer 19"</t>
   </si>
   <si>
-    <t>Lt. 5</t>
-  </si>
-  <si>
     <t>Intan</t>
   </si>
   <si>
     <t>ASRock H61M-VG3</t>
   </si>
   <si>
-    <t>Lt. 6</t>
-  </si>
-  <si>
     <t>Alisa</t>
   </si>
   <si>
@@ -199,9 +187,6 @@
     <t>Intel G31</t>
   </si>
   <si>
-    <t>Lt. 7</t>
-  </si>
-  <si>
     <t>Engineering</t>
   </si>
   <si>
@@ -211,7 +196,7 @@
     <t>Core i3 - 2100, 3.1GHz</t>
   </si>
   <si>
-    <t>12 GB</t>
+    <t>12GB</t>
   </si>
   <si>
     <t>Nvidia Gforce 8400GS</t>
@@ -223,7 +208,7 @@
     <t>Core 2 Duo E7500</t>
   </si>
   <si>
-    <t>8 GB</t>
+    <t>8GB</t>
   </si>
   <si>
     <t>Dell 19"</t>
@@ -232,7 +217,7 @@
     <t>Print Server</t>
   </si>
   <si>
-    <t>4 GB</t>
+    <t>4GB</t>
   </si>
   <si>
     <t>-</t>
@@ -304,18 +289,45 @@
     <t>Core i7 3.6GHz HZ77</t>
   </si>
   <si>
+    <t>Purwiyono</t>
+  </si>
+  <si>
+    <t>HP Prodesk 400 G5</t>
+  </si>
+  <si>
+    <t>Core i7 3.6GHz HZ78</t>
+  </si>
+  <si>
+    <t>Nvidia Gforce GT730 3GB</t>
+  </si>
+  <si>
+    <t>Win 10 65Bit</t>
+  </si>
+  <si>
+    <t>Nvidia Gforce 210</t>
+  </si>
+  <si>
+    <t>LG 23"</t>
+  </si>
+  <si>
+    <t>MSI H55M-E32</t>
+  </si>
+  <si>
+    <t>Core i5 650, 3.1GHz</t>
+  </si>
+  <si>
+    <t>Intel H55M</t>
+  </si>
+  <si>
+    <t>MSI G41M-P28</t>
+  </si>
+  <si>
     <t>Eko</t>
   </si>
   <si>
     <t>QC</t>
   </si>
   <si>
-    <t>MSI G41M-P28</t>
-  </si>
-  <si>
-    <t>2GB</t>
-  </si>
-  <si>
     <t>Intel G41</t>
   </si>
   <si>
@@ -331,9 +343,6 @@
     <t>Dedi</t>
   </si>
   <si>
-    <t>1GB</t>
-  </si>
-  <si>
     <t>Yuli</t>
   </si>
   <si>
@@ -352,6 +361,15 @@
     <t>Pentium G620</t>
   </si>
   <si>
+    <t>Dimas</t>
+  </si>
+  <si>
+    <t>MSI G41M-P33 Combo</t>
+  </si>
+  <si>
+    <t>Dual Core E5700</t>
+  </si>
+  <si>
     <t>Tanti</t>
   </si>
   <si>
@@ -367,7 +385,13 @@
     <t>Dyah</t>
   </si>
   <si>
-    <t>4GB</t>
+    <t>Dimyati</t>
+  </si>
+  <si>
+    <t>Muis</t>
+  </si>
+  <si>
+    <t>Udin</t>
   </si>
   <si>
     <t>Wito</t>
@@ -392,6 +416,60 @@
   </si>
   <si>
     <t>LG 19”</t>
+  </si>
+  <si>
+    <t>ex. Retno</t>
+  </si>
+  <si>
+    <t>Risca</t>
+  </si>
+  <si>
+    <t>HRD</t>
+  </si>
+  <si>
+    <t>WIN 7 64Bit</t>
+  </si>
+  <si>
+    <t>Khanza</t>
+  </si>
+  <si>
+    <t>WIN 7 32Bit</t>
+  </si>
+  <si>
+    <t>Hidayat</t>
+  </si>
+  <si>
+    <t>Produksi</t>
+  </si>
+  <si>
+    <t>MSI H61M-P20(G3)</t>
+  </si>
+  <si>
+    <t>Core I3-2100 3.10GHz</t>
+  </si>
+  <si>
+    <t>GeForce 210</t>
+  </si>
+  <si>
+    <t>Hafid</t>
+  </si>
+  <si>
+    <t>GeForce 8400GS</t>
+  </si>
+  <si>
+    <t>Iswandi</t>
+  </si>
+  <si>
+    <t>Produksi/Packing</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Lutfi/Fauzi/Zakaria</t>
+  </si>
+  <si>
+    <t>Pentium G2030</t>
   </si>
 </sst>
 </file>
@@ -399,12 +477,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #.##0_);_(* \(#.##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_(* #,###.##000_);_(* \(#,###.##000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,###.##000_);_(* \(#,###.##000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #.##0_);_(* \(#.##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,12 +493,24 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="0"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -441,18 +531,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -465,12 +585,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -478,26 +599,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -524,40 +630,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -572,7 +655,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,13 +781,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -602,31 +799,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -644,115 +823,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -781,6 +864,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -801,30 +893,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -859,11 +927,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -878,160 +952,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1043,6 +1126,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1364,10 +1450,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1684,7 +1770,7 @@
         <v>161</v>
       </c>
       <c r="N7" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="O7" t="s">
         <v>27</v>
@@ -1695,7 +1781,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
         <v>45</v>
@@ -1722,7 +1808,7 @@
         <v>23</v>
       </c>
       <c r="K8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L8" t="s">
         <v>39</v>
@@ -1731,7 +1817,7 @@
         <v>164</v>
       </c>
       <c r="N8" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="O8" t="s">
         <v>27</v>
@@ -1742,7 +1828,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
         <v>45</v>
@@ -1754,7 +1840,7 @@
         <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G9" t="s">
         <v>38</v>
@@ -1763,7 +1849,7 @@
         <v>250</v>
       </c>
       <c r="I9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J9" t="s">
         <v>24</v>
@@ -1778,7 +1864,7 @@
         <v>166</v>
       </c>
       <c r="N9" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="O9" t="s">
         <v>27</v>
@@ -1789,13 +1875,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
         <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
         <v>37</v>
@@ -1810,7 +1896,7 @@
         <v>320</v>
       </c>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J10" t="s">
         <v>23</v>
@@ -1825,7 +1911,7 @@
         <v>163</v>
       </c>
       <c r="N10" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="O10" t="s">
         <v>27</v>
@@ -1836,34 +1922,34 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H11">
         <v>250</v>
       </c>
       <c r="I11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J11" t="s">
         <v>23</v>
       </c>
       <c r="K11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L11" t="s">
         <v>39</v>
@@ -1872,7 +1958,7 @@
         <v>162</v>
       </c>
       <c r="N11" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="O11" t="s">
         <v>27</v>
@@ -1883,22 +1969,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H12">
         <v>250</v>
@@ -1930,19 +2016,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
         <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G13" t="s">
         <v>38</v>
@@ -1951,7 +2037,7 @@
         <v>250</v>
       </c>
       <c r="I13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J13" t="s">
         <v>23</v>
@@ -1977,19 +2063,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
         <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G14" t="s">
         <v>21</v>
@@ -2001,7 +2087,7 @@
         <v>22</v>
       </c>
       <c r="J14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="K14" t="s">
         <v>24</v>
@@ -2024,34 +2110,34 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" t="s">
         <v>64</v>
       </c>
-      <c r="F15" t="s">
-        <v>69</v>
-      </c>
       <c r="G15" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H15">
         <v>250</v>
       </c>
       <c r="I15" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J15" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="K15" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="L15" t="s">
         <v>25</v>
@@ -2071,37 +2157,37 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G16" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H16">
         <v>1000</v>
       </c>
       <c r="I16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J16" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" t="s">
+        <v>71</v>
+      </c>
+      <c r="L16" t="s">
         <v>76</v>
-      </c>
-      <c r="K16" t="s">
-        <v>76</v>
-      </c>
-      <c r="L16" t="s">
-        <v>81</v>
       </c>
       <c r="M16">
         <v>17</v>
@@ -2118,37 +2204,37 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
         <v>78</v>
       </c>
-      <c r="E17" t="s">
-        <v>83</v>
-      </c>
       <c r="F17" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H17">
         <v>1000</v>
       </c>
       <c r="I17" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J17" t="s">
+        <v>71</v>
+      </c>
+      <c r="K17" t="s">
+        <v>71</v>
+      </c>
+      <c r="L17" t="s">
         <v>76</v>
-      </c>
-      <c r="K17" t="s">
-        <v>76</v>
-      </c>
-      <c r="L17" t="s">
-        <v>81</v>
       </c>
       <c r="M17">
         <v>36</v>
@@ -2165,37 +2251,37 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G18" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H18">
         <v>1000</v>
       </c>
       <c r="I18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J18" t="s">
+        <v>71</v>
+      </c>
+      <c r="K18" t="s">
+        <v>71</v>
+      </c>
+      <c r="L18" t="s">
         <v>76</v>
-      </c>
-      <c r="K18" t="s">
-        <v>76</v>
-      </c>
-      <c r="L18" t="s">
-        <v>81</v>
       </c>
       <c r="M18">
         <v>27</v>
@@ -2212,37 +2298,37 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F19" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H19">
         <v>1000</v>
       </c>
       <c r="I19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J19" t="s">
+        <v>71</v>
+      </c>
+      <c r="K19" t="s">
+        <v>71</v>
+      </c>
+      <c r="L19" t="s">
         <v>76</v>
-      </c>
-      <c r="K19" t="s">
-        <v>76</v>
-      </c>
-      <c r="L19" t="s">
-        <v>81</v>
       </c>
       <c r="M19">
         <v>24</v>
@@ -2259,37 +2345,37 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F20" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G20" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H20">
         <v>1000</v>
       </c>
       <c r="I20" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J20" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" t="s">
+        <v>71</v>
+      </c>
+      <c r="L20" t="s">
         <v>76</v>
-      </c>
-      <c r="K20" t="s">
-        <v>76</v>
-      </c>
-      <c r="L20" t="s">
-        <v>81</v>
       </c>
       <c r="M20">
         <v>12</v>
@@ -2306,37 +2392,37 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H21">
         <v>1000</v>
       </c>
       <c r="I21" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J21" t="s">
+        <v>71</v>
+      </c>
+      <c r="K21" t="s">
+        <v>71</v>
+      </c>
+      <c r="L21" t="s">
         <v>76</v>
-      </c>
-      <c r="K21" t="s">
-        <v>76</v>
-      </c>
-      <c r="L21" t="s">
-        <v>81</v>
       </c>
       <c r="M21">
         <v>31</v>
@@ -2353,37 +2439,37 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F22" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H22">
         <v>1000</v>
       </c>
       <c r="I22" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J22" t="s">
+        <v>71</v>
+      </c>
+      <c r="K22" t="s">
+        <v>71</v>
+      </c>
+      <c r="L22" t="s">
         <v>76</v>
-      </c>
-      <c r="K22" t="s">
-        <v>76</v>
-      </c>
-      <c r="L22" t="s">
-        <v>81</v>
       </c>
       <c r="M22">
         <v>15</v>
@@ -2400,37 +2486,37 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H23">
         <v>1000</v>
       </c>
       <c r="I23" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J23" t="s">
+        <v>71</v>
+      </c>
+      <c r="K23" t="s">
+        <v>71</v>
+      </c>
+      <c r="L23" t="s">
         <v>76</v>
-      </c>
-      <c r="K23" t="s">
-        <v>76</v>
-      </c>
-      <c r="L23" t="s">
-        <v>81</v>
       </c>
       <c r="M23">
         <v>38</v>
@@ -2442,30 +2528,233 @@
         <v>27</v>
       </c>
     </row>
+    <row r="24" spans="2:15">
+      <c r="B24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24">
+        <v>1000</v>
+      </c>
+      <c r="I24" t="s">
+        <v>70</v>
+      </c>
+      <c r="J24" t="s">
+        <v>71</v>
+      </c>
+      <c r="K24" t="s">
+        <v>71</v>
+      </c>
+      <c r="L24" t="s">
+        <v>95</v>
+      </c>
+      <c r="M24"/>
+      <c r="N24" t="s">
+        <v>26</v>
+      </c>
+      <c r="O24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15">
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H25">
+        <v>184</v>
+      </c>
+      <c r="I25" t="s">
+        <v>97</v>
+      </c>
+      <c r="J25" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" t="s">
+        <v>23</v>
+      </c>
+      <c r="L25" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25">
+        <v>13</v>
+      </c>
+      <c r="N25" t="s">
+        <v>26</v>
+      </c>
+      <c r="O25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15">
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" t="s">
+        <v>100</v>
+      </c>
+      <c r="H26">
+        <v>250</v>
+      </c>
+      <c r="I26" t="s">
+        <v>70</v>
+      </c>
+      <c r="J26" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" t="s">
+        <v>71</v>
+      </c>
+      <c r="L26" t="s">
+        <v>25</v>
+      </c>
+      <c r="M26">
+        <v>39</v>
+      </c>
+      <c r="N26" t="s">
+        <v>26</v>
+      </c>
+      <c r="O26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15">
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27">
+        <v>250</v>
+      </c>
+      <c r="I27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" t="s">
+        <v>71</v>
+      </c>
+      <c r="K27" t="s">
+        <v>71</v>
+      </c>
+      <c r="L27" t="s">
+        <v>39</v>
+      </c>
+      <c r="M27">
+        <v>37</v>
+      </c>
+      <c r="N27" t="s">
+        <v>26</v>
+      </c>
+      <c r="O27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15">
+      <c r="D28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" t="s">
+        <v>60</v>
+      </c>
+      <c r="G28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28">
+        <v>184</v>
+      </c>
+      <c r="I28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" t="s">
+        <v>23</v>
+      </c>
+      <c r="L28" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28">
+        <v>30</v>
+      </c>
+      <c r="N28" t="s">
+        <v>26</v>
+      </c>
+      <c r="O28" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="31" spans="2:15">
       <c r="B31" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H31" s="2">
         <v>320</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>23</v>
@@ -2480,7 +2769,7 @@
         <v>85</v>
       </c>
       <c r="N31" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="O31" t="s">
         <v>27</v>
@@ -2488,28 +2777,28 @@
     </row>
     <row r="32" spans="2:15">
       <c r="B32" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H32" s="2">
         <v>250</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>23</v>
@@ -2524,7 +2813,7 @@
         <v>84</v>
       </c>
       <c r="N32" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="O32" t="s">
         <v>27</v>
@@ -2532,28 +2821,28 @@
     </row>
     <row r="33" spans="2:15">
       <c r="B33" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>105</v>
+        <v>49</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H33" s="2">
         <v>250</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>23</v>
@@ -2568,7 +2857,7 @@
         <v>83</v>
       </c>
       <c r="N33" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="O33" t="s">
         <v>27</v>
@@ -2576,22 +2865,22 @@
     </row>
     <row r="34" spans="2:15">
       <c r="B34" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H34" s="2">
         <v>250</v>
@@ -2612,7 +2901,7 @@
         <v>84</v>
       </c>
       <c r="N34" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="O34" t="s">
         <v>27</v>
@@ -2620,19 +2909,19 @@
     </row>
     <row r="35" spans="2:15">
       <c r="B35" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>21</v>
@@ -2641,7 +2930,7 @@
         <v>250</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>24</v>
@@ -2656,229 +2945,754 @@
         <v>86</v>
       </c>
       <c r="N35" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="O35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="2:15">
-      <c r="B37" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E37" t="s">
-        <v>37</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H37">
+    <row r="36" spans="2:15">
+      <c r="B36" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H36" s="2">
         <v>250</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L37" t="s">
+      <c r="I36" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" t="s">
+        <v>23</v>
+      </c>
+      <c r="L36" t="s">
         <v>33</v>
       </c>
-      <c r="M37">
-        <v>76</v>
-      </c>
-      <c r="N37" t="s">
-        <v>101</v>
-      </c>
-      <c r="O37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="2:15">
-      <c r="B38" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E38" t="s">
-        <v>37</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H38">
-        <v>250</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L38" t="s">
-        <v>39</v>
-      </c>
-      <c r="M38">
-        <v>78</v>
-      </c>
-      <c r="N38" t="s">
-        <v>101</v>
-      </c>
-      <c r="O38" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="2:15">
-      <c r="B39" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E39" t="s">
-        <v>37</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H39">
-        <v>320</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L39" t="s">
-        <v>25</v>
-      </c>
-      <c r="M39">
-        <v>189</v>
-      </c>
-      <c r="N39" t="s">
-        <v>101</v>
-      </c>
-      <c r="O39" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="2:15">
-      <c r="B41" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E41" t="s">
-        <v>30</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41">
-        <v>500</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L41" t="s">
-        <v>25</v>
-      </c>
-      <c r="M41">
-        <v>113</v>
-      </c>
-      <c r="N41" t="s">
-        <v>101</v>
-      </c>
-      <c r="O41" t="s">
+      <c r="M36">
+        <v>124</v>
+      </c>
+      <c r="N36" t="s">
+        <v>105</v>
+      </c>
+      <c r="O36" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="43" spans="2:15">
       <c r="B43" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
+      </c>
+      <c r="E43" t="s">
+        <v>37</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H43">
         <v>250</v>
       </c>
       <c r="I43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L43" t="s">
+        <v>33</v>
+      </c>
+      <c r="M43">
+        <v>76</v>
+      </c>
+      <c r="N43" t="s">
+        <v>105</v>
+      </c>
+      <c r="O43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15">
+      <c r="B44" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E44" t="s">
+        <v>37</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H44">
+        <v>250</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L44" t="s">
+        <v>39</v>
+      </c>
+      <c r="M44">
+        <v>78</v>
+      </c>
+      <c r="N44" t="s">
+        <v>105</v>
+      </c>
+      <c r="O44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15">
+      <c r="B45" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H45">
+        <v>320</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L45" t="s">
+        <v>25</v>
+      </c>
+      <c r="M45">
+        <v>189</v>
+      </c>
+      <c r="N45" t="s">
+        <v>105</v>
+      </c>
+      <c r="O45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15">
+      <c r="B46" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H46" s="4">
+        <v>250</v>
+      </c>
+      <c r="I46" t="s">
+        <v>22</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L46" t="s">
+        <v>39</v>
+      </c>
+      <c r="M46">
+        <v>77</v>
+      </c>
+      <c r="N46" t="s">
+        <v>105</v>
+      </c>
+      <c r="O46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15">
+      <c r="B47" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H47" s="4">
+        <v>250</v>
+      </c>
+      <c r="I47" t="s">
+        <v>50</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L47" t="s">
+        <v>39</v>
+      </c>
+      <c r="M47">
+        <v>79</v>
+      </c>
+      <c r="N47" t="s">
+        <v>105</v>
+      </c>
+      <c r="O47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15">
+      <c r="B48" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J43" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L43" t="s">
+      <c r="C48" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H48" s="4">
+        <v>250</v>
+      </c>
+      <c r="I48" t="s">
+        <v>22</v>
+      </c>
+      <c r="J48" t="s">
+        <v>24</v>
+      </c>
+      <c r="K48" t="s">
+        <v>24</v>
+      </c>
+      <c r="L48" t="s">
         <v>39</v>
       </c>
-      <c r="M43">
+      <c r="M48">
+        <v>75</v>
+      </c>
+      <c r="N48" t="s">
+        <v>105</v>
+      </c>
+      <c r="O48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15">
+      <c r="B56" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E56" t="s">
+        <v>30</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H56">
+        <v>500</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L56" t="s">
+        <v>25</v>
+      </c>
+      <c r="M56">
+        <v>113</v>
+      </c>
+      <c r="N56" t="s">
+        <v>105</v>
+      </c>
+      <c r="O56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="2:15">
+      <c r="B62" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H62">
+        <v>250</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L62" t="s">
+        <v>39</v>
+      </c>
+      <c r="M62">
         <v>233</v>
       </c>
-      <c r="N43" t="s">
-        <v>101</v>
-      </c>
-      <c r="O43" t="s">
+      <c r="N62" t="s">
+        <v>105</v>
+      </c>
+      <c r="O62" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="2:15">
+      <c r="B63" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H63" s="4">
+        <v>250</v>
+      </c>
+      <c r="I63" t="s">
+        <v>22</v>
+      </c>
+      <c r="J63" t="s">
+        <v>23</v>
+      </c>
+      <c r="K63" t="s">
+        <v>23</v>
+      </c>
+      <c r="L63" t="s">
+        <v>33</v>
+      </c>
+      <c r="N63" t="s">
+        <v>105</v>
+      </c>
+      <c r="O63" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70" spans="2:15">
+      <c r="B70" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H70">
+        <v>500</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K70" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L70" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="M70">
+        <v>96</v>
+      </c>
+      <c r="N70" t="s">
+        <v>105</v>
+      </c>
+      <c r="O70" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="2:15">
+      <c r="B71" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H71">
+        <v>500</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K71" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L71" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="M71">
+        <v>63</v>
+      </c>
+      <c r="N71" t="s">
+        <v>105</v>
+      </c>
+      <c r="O71" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="78" spans="2:15">
+      <c r="B78" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="H78" s="4">
+        <v>250</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J78" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K78" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L78" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="M78">
+        <v>127</v>
+      </c>
+      <c r="N78" t="s">
+        <v>105</v>
+      </c>
+      <c r="O78" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="2:15">
+      <c r="B79" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H79" s="4">
+        <v>250</v>
+      </c>
+      <c r="I79" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K79" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L79" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="M79">
+        <v>122</v>
+      </c>
+      <c r="N79" t="s">
+        <v>105</v>
+      </c>
+      <c r="O79" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="2:15">
+      <c r="B80" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H80" s="4">
+        <v>250</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K80" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L80" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M80">
+        <v>133</v>
+      </c>
+      <c r="N80" t="s">
+        <v>105</v>
+      </c>
+      <c r="O80" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="2:15">
+      <c r="B81" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H81" s="4">
+        <v>250</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K81" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L81" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M81">
+        <v>61</v>
+      </c>
+      <c r="N81" t="s">
+        <v>105</v>
+      </c>
+      <c r="O81" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="2:15">
+      <c r="B82" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H82" s="4">
+        <v>250</v>
+      </c>
+      <c r="I82" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K82" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L82" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M82">
+        <v>58</v>
+      </c>
+      <c r="N82" t="s">
+        <v>105</v>
+      </c>
+      <c r="O82" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>